<commit_message>
Minor styling adjustments + Update readme.md
</commit_message>
<xml_diff>
--- a/Site-Testing/Manual-User Testing-Case.xlsx
+++ b/Site-Testing/Manual-User Testing-Case.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanchoi/Desktop/JORDAN CHOI/Education/Ngee Ann Polytechnic/Academic/Semester 1.2/Interactive Development (IMGD 1_ID P01)/Assignments &amp; Tests/Assignment 2/ID_S10208161D_JordanChoi_Assg2/Manual User Testing Case/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanchoi/Desktop/JORDAN CHOI/Education/Ngee Ann Polytechnic/Academic/Semester 1.2/Interactive Development (IMGD 1_ID P01)/Assignments &amp; Tests/Assignment 2/ID_S10208161D_JordanChoi_Assg2/Site-Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94706A1B-779E-F843-A13C-36D3C0E30DD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731F0A77-2B30-B740-A46C-EE429A13DAC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Desktop" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="79">
   <si>
     <t>Test #</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>Mobile Menu Expands and Displayed</t>
+  </si>
+  <si>
+    <t>Preloader is shown with animated message and images, then fades out</t>
   </si>
 </sst>
 </file>
@@ -631,8 +634,8 @@
   </sheetPr>
   <dimension ref="A1:Z1046"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -713,7 +716,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
     </row>
-    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:26" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -721,10 +724,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>6</v>
@@ -752,14 +755,22 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
+      <c r="A4" s="15">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="7"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -781,23 +792,15 @@
       <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
     </row>
-    <row r="5" spans="1:26" ht="28" x14ac:dyDescent="0.15">
-      <c r="A5" s="15">
-        <v>2</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="7"/>
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A5" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -824,13 +827,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>6</v>
@@ -862,13 +865,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>6</v>
@@ -900,13 +903,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>6</v>
@@ -933,15 +936,23 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
-      <c r="A9" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+    <row r="9" spans="1:26" ht="28" x14ac:dyDescent="0.15">
+      <c r="A9" s="15">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="7"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -963,23 +974,15 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" ht="28" x14ac:dyDescent="0.15">
-      <c r="A10" s="15">
-        <v>6</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="7"/>
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1005,14 +1008,14 @@
       <c r="A11" s="15">
         <v>7</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>21</v>
+      <c r="B11" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>6</v>
@@ -1043,14 +1046,14 @@
       <c r="A12" s="15">
         <v>8</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>23</v>
+      <c r="B12" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>6</v>
@@ -1082,13 +1085,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>6</v>
@@ -1119,14 +1122,14 @@
       <c r="A14" s="15">
         <v>10</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>25</v>
+      <c r="B14" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>6</v>
@@ -1153,15 +1156,23 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26" ht="14" x14ac:dyDescent="0.15">
-      <c r="A15" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
+    <row r="15" spans="1:26" ht="28" x14ac:dyDescent="0.15">
+      <c r="A15" s="15">
+        <v>11</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="7"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -1183,23 +1194,15 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26" ht="28" x14ac:dyDescent="0.15">
-      <c r="A16" s="15">
-        <v>11</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="7"/>
+    <row r="16" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A16" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -1226,13 +1229,13 @@
         <v>12</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>6</v>
@@ -1264,13 +1267,13 @@
         <v>13</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>6</v>
@@ -1302,18 +1305,18 @@
         <v>14</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E19" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="18"/>
+      <c r="F19" s="7"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -1340,13 +1343,13 @@
         <v>15</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" s="16" t="s">
         <v>6</v>
@@ -1378,18 +1381,18 @@
         <v>16</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E21" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="7"/>
+      <c r="F21" s="18"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -1411,15 +1414,23 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A22" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+    <row r="22" spans="1:26" ht="28" x14ac:dyDescent="0.15">
+      <c r="A22" s="15">
+        <v>17</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="7"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -1441,23 +1452,15 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" ht="28" x14ac:dyDescent="0.15">
-      <c r="A23" s="6">
-        <v>17</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="18"/>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A23" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -1479,18 +1482,18 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24" spans="1:26" ht="42" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:26" ht="28" x14ac:dyDescent="0.15">
       <c r="A24" s="6">
         <v>18</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E24" s="16" t="s">
         <v>6</v>
@@ -1517,15 +1520,23 @@
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A25" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
+    <row r="25" spans="1:26" ht="42" x14ac:dyDescent="0.15">
+      <c r="A25" s="6">
+        <v>19</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="18"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -1547,23 +1558,15 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
     </row>
-    <row r="26" spans="1:26" ht="28" x14ac:dyDescent="0.15">
-      <c r="A26" s="6">
-        <v>20</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="7"/>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
@@ -1585,18 +1588,18 @@
       <c r="Y26" s="8"/>
       <c r="Z26" s="8"/>
     </row>
-    <row r="27" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:26" ht="28" x14ac:dyDescent="0.15">
       <c r="A27" s="6">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E27" s="16" t="s">
         <v>6</v>
@@ -1625,10 +1628,10 @@
     </row>
     <row r="28" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="6">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>48</v>
@@ -1663,10 +1666,10 @@
     </row>
     <row r="29" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="6">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>48</v>
@@ -1677,7 +1680,7 @@
       <c r="E29" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F29" s="18"/>
+      <c r="F29" s="7"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
@@ -1701,10 +1704,10 @@
     </row>
     <row r="30" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="6">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>48</v>
@@ -1737,15 +1740,23 @@
       <c r="Y30" s="8"/>
       <c r="Z30" s="8"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A31" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
+    <row r="31" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A31" s="6">
+        <v>24</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="18"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
@@ -1767,23 +1778,15 @@
       <c r="Y31" s="8"/>
       <c r="Z31" s="8"/>
     </row>
-    <row r="32" spans="1:26" ht="14" x14ac:dyDescent="0.15">
-      <c r="A32" s="6">
-        <v>25</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F32" s="3"/>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A32" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
@@ -1805,18 +1808,18 @@
       <c r="Y32" s="8"/>
       <c r="Z32" s="8"/>
     </row>
-    <row r="33" spans="1:26" ht="28" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="6">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>6</v>
@@ -1845,16 +1848,16 @@
     </row>
     <row r="34" spans="1:26" ht="28" x14ac:dyDescent="0.15">
       <c r="A34" s="6">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E34" s="11" t="s">
         <v>6</v>
@@ -1883,16 +1886,16 @@
     </row>
     <row r="35" spans="1:26" ht="28" x14ac:dyDescent="0.15">
       <c r="A35" s="6">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E35" s="11" t="s">
         <v>6</v>
@@ -1919,18 +1922,18 @@
       <c r="Y35" s="8"/>
       <c r="Z35" s="8"/>
     </row>
-    <row r="36" spans="1:26" ht="42" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:26" ht="28" x14ac:dyDescent="0.15">
       <c r="A36" s="6">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>62</v>
+        <v>59</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>6</v>
@@ -1957,15 +1960,23 @@
       <c r="Y36" s="8"/>
       <c r="Z36" s="8"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A37" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
+    <row r="37" spans="1:26" ht="42" x14ac:dyDescent="0.15">
+      <c r="A37" s="6">
+        <v>29</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" s="3"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
@@ -1987,23 +1998,15 @@
       <c r="Y37" s="8"/>
       <c r="Z37" s="8"/>
     </row>
-    <row r="38" spans="1:26" ht="14" x14ac:dyDescent="0.15">
-      <c r="A38" s="6">
-        <v>34</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F38" s="3"/>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A38" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
@@ -2025,18 +2028,18 @@
       <c r="Y38" s="8"/>
       <c r="Z38" s="8"/>
     </row>
-    <row r="39" spans="1:26" ht="28" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="6">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E39" s="11" t="s">
         <v>6</v>
@@ -2065,16 +2068,16 @@
     </row>
     <row r="40" spans="1:26" ht="28" x14ac:dyDescent="0.15">
       <c r="A40" s="6">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>6</v>
@@ -2101,18 +2104,18 @@
       <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
     </row>
-    <row r="41" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:26" ht="28" x14ac:dyDescent="0.15">
       <c r="A41" s="6">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>6</v>
@@ -2139,15 +2142,23 @@
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A42" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
+    <row r="42" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A42" s="6">
+        <v>33</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
@@ -2169,23 +2180,15 @@
       <c r="Y42" s="3"/>
       <c r="Z42" s="3"/>
     </row>
-    <row r="43" spans="1:26" ht="14" x14ac:dyDescent="0.15">
-      <c r="A43" s="6">
-        <v>38</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F43" s="3"/>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A43" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -2207,12 +2210,22 @@
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
+    <row r="44" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A44" s="6">
+        <v>34</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -2656,12 +2669,12 @@
       <c r="Z59" s="3"/>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A60" s="10"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
@@ -2740,12 +2753,12 @@
       <c r="Z62" s="3"/>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
+      <c r="A63" s="10"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
@@ -2908,12 +2921,12 @@
       <c r="Z68" s="3"/>
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A69" s="10"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="10"/>
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
@@ -2936,12 +2949,12 @@
       <c r="Z69" s="3"/>
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
+      <c r="A70" s="10"/>
+      <c r="B70" s="10"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
@@ -26960,6 +26973,12 @@
       <c r="Z927" s="3"/>
     </row>
     <row r="928" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A928" s="3"/>
+      <c r="B928" s="3"/>
+      <c r="C928" s="3"/>
+      <c r="D928" s="3"/>
+      <c r="E928" s="3"/>
+      <c r="F928" s="3"/>
       <c r="G928" s="3"/>
       <c r="H928" s="3"/>
       <c r="I928" s="3"/>
@@ -29588,10 +29607,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="37.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -29626,7 +29645,7 @@
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
     </row>
-    <row r="3" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -29634,10 +29653,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>6</v>
@@ -29645,45 +29664,45 @@
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="15">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="1:6" ht="42" x14ac:dyDescent="0.15">
-      <c r="A5" s="15">
-        <v>2</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="7"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A6" s="15">
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>6</v>
@@ -29695,13 +29714,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>6</v>
@@ -29713,59 +29732,59 @@
         <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+      <c r="A9" s="15">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" spans="1:6" ht="42" x14ac:dyDescent="0.15">
-      <c r="A10" s="15">
-        <v>6</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="7"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A11" s="15">
         <v>7</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>21</v>
+      <c r="B11" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>6</v>
@@ -29776,14 +29795,14 @@
       <c r="A12" s="15">
         <v>8</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>23</v>
+      <c r="B12" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>6</v>
@@ -29795,13 +29814,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>6</v>
@@ -29812,60 +29831,60 @@
       <c r="A14" s="15">
         <v>10</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>25</v>
+      <c r="B14" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A15" s="17" t="s">
+    <row r="15" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+      <c r="A15" s="15">
+        <v>11</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A16" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="1:6" ht="28" x14ac:dyDescent="0.15">
-      <c r="A16" s="15">
-        <v>11</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="7"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A17" s="15">
         <v>12</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>6</v>
@@ -29877,13 +29896,13 @@
         <v>13</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>6</v>
@@ -29895,31 +29914,31 @@
         <v>14</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E19" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="18"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A20" s="15">
         <v>15</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" s="16" t="s">
         <v>6</v>
@@ -29931,105 +29950,105 @@
         <v>16</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E21" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="7"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A22" s="9" t="s">
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A22" s="15">
+        <v>17</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" ht="28" x14ac:dyDescent="0.15">
-      <c r="A23" s="6">
-        <v>17</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="18"/>
-    </row>
-    <row r="24" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A24" s="6">
         <v>18</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E24" s="16" t="s">
         <v>6</v>
       </c>
       <c r="F24" s="18"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25" s="9" t="s">
+    <row r="25" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+      <c r="A25" s="6">
+        <v>19</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" ht="28" x14ac:dyDescent="0.15">
-      <c r="A26" s="6">
-        <v>20</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="7"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A27" s="6">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E27" s="16" t="s">
         <v>6</v>
@@ -30038,10 +30057,10 @@
     </row>
     <row r="28" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A28" s="6">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>48</v>
@@ -30056,10 +30075,10 @@
     </row>
     <row r="29" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A29" s="6">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>48</v>
@@ -30070,14 +30089,14 @@
       <c r="E29" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F29" s="18"/>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A30" s="6">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>48</v>
@@ -30090,46 +30109,46 @@
       </c>
       <c r="F30" s="18"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A31" s="9" t="s">
+    <row r="31" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A31" s="6">
+        <v>24</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="18"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:6" ht="28" x14ac:dyDescent="0.15">
-      <c r="A32" s="6">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A33" s="6">
         <v>25</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B33" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C33" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" ht="42" x14ac:dyDescent="0.15">
-      <c r="A33" s="6">
-        <v>26</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>56</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>6</v>
@@ -30138,16 +30157,16 @@
     </row>
     <row r="34" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A34" s="6">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E34" s="11" t="s">
         <v>6</v>
@@ -30156,16 +30175,16 @@
     </row>
     <row r="35" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A35" s="6">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E35" s="11" t="s">
         <v>6</v>
@@ -30174,80 +30193,80 @@
     </row>
     <row r="36" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A36" s="6">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>62</v>
+        <v>59</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+      <c r="A37" s="6">
+        <v>29</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A38" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-    </row>
-    <row r="38" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A38" s="6">
-        <v>34</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F38" s="3"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="6">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="E39" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="6">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>6</v>
@@ -30256,16 +30275,16 @@
     </row>
     <row r="41" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A41" s="6">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>6</v>
@@ -30274,49 +30293,67 @@
     </row>
     <row r="42" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A42" s="6">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A43" s="9" t="s">
+    <row r="43" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A43" s="6">
+        <v>34</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A44" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-    </row>
-    <row r="44" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A44" s="6">
-        <v>42</v>
-      </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A45" s="6">
+        <v>35</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C45" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D45" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="E45" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F44" s="3"/>
+      <c r="F45" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>